<commit_message>
Commit on November 23, 2021
</commit_message>
<xml_diff>
--- a/Research Stats.xlsx
+++ b/Research Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbouillon/Git/research_tlds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAF0A6D-0CCC-2D4D-8BAC-EECC3FA19167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75321826-48E4-6A40-813B-D7DE0F9C5429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-39840" yWindow="5040" windowWidth="28040" windowHeight="17440" xr2:uid="{8AAD0516-B722-DE45-B573-02C4ECF95119}"/>
+    <workbookView xWindow="-39840" yWindow="5040" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{8AAD0516-B722-DE45-B573-02C4ECF95119}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -49,12 +49,6 @@
     <t>Browser Breakdown</t>
   </si>
   <si>
-    <t>/restapi.php</t>
-  </si>
-  <si>
-    <t>iOS 15.02</t>
-  </si>
-  <si>
     <t>Mobile Safari</t>
   </si>
   <si>
@@ -86,6 +80,72 @@
   </si>
   <si>
     <t>Chrome 83</t>
+  </si>
+  <si>
+    <t>Windows 10 62.5% / 12.5% - Vista</t>
+  </si>
+  <si>
+    <t>No views from within California  - 5 from Boardman, Oregon, the remaining requests from other countries.</t>
+  </si>
+  <si>
+    <t>Windows 10</t>
+  </si>
+  <si>
+    <t>Chrome 78</t>
+  </si>
+  <si>
+    <t>2 Views from CA bay area, 2 from Kansas, the rest other countries</t>
+  </si>
+  <si>
+    <t>Windows</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
+    <t>No views from within California - 50% of views are from Boardman again - This is strange.</t>
+  </si>
+  <si>
+    <t>1 view from Southern California (LA), Boardman 2 views</t>
+  </si>
+  <si>
+    <t>November 20-23</t>
+  </si>
+  <si>
+    <t>Network Events</t>
+  </si>
+  <si>
+    <t>Unique Private Ips</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Source Ips</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
   </si>
 </sst>
 </file>
@@ -451,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDF59B2B-A2AA-8D4F-87B1-5D5944105DF8}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -481,16 +541,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -498,16 +558,16 @@
         <v>44517</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3">
         <v>0.48959999999999998</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2" s="3">
         <v>0.56969999999999998</v>
@@ -521,22 +581,22 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
         <v>0.75</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" s="3">
         <v>0.28570000000000001</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -544,7 +604,103 @@
         <v>44519</v>
       </c>
       <c r="B4" s="6">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.28570000000000001</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>44520</v>
+      </c>
+      <c r="B5" s="6">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>44521</v>
+      </c>
+      <c r="B6" s="6">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.77780000000000005</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>44522</v>
+      </c>
+      <c r="B7" s="6">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.85709999999999997</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -554,58 +710,107 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5A93F00-4044-0A4E-86C6-B1B0B97CDB7E}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="2" width="30.5" customWidth="1"/>
-    <col min="3" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>602</v>
+      </c>
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>44518</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8">
         <v>5</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.5161</v>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>